<commit_message>
further development with allocations and return values
</commit_message>
<xml_diff>
--- a/data/各区域边界经纬度.xlsx
+++ b/data/各区域边界经纬度.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2019春夏学期\运筹学与系统工程\大作业\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Terence\Documents\Senior2\OperationsResearchNSystemsEngineering\ZJGarbageProgram\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21D0741F-631D-49FE-82BE-E22D92C8FEC0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7C4230-CAAF-445A-B592-24A119A67775}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9012" xr2:uid="{580764D7-2A58-4E62-A68D-9F24D0685060}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{580764D7-2A58-4E62-A68D-9F24D0685060}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>地理位置名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -55,10 +60,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>休闲风味</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>翠柏</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -99,18 +100,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>生命科学研究院</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>医药学院</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>金工化学实验中心</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>西教学区</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -128,6 +117,30 @@
   </si>
   <si>
     <t>说明：每个区域抽象为四边形区域，1，2，3，4为四对经纬度点。因为四点对应可能是任意的一个四边形，所以不能简单的用矩阵方式来计算区域内的人数之和。（也许可以转化为平面二维坐标来做）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>经度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>纬度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大食堂</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>医学院药学院</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>纳米楼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>金工化学生物</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -186,7 +199,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -202,7 +215,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -501,7 +514,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -521,7 +534,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -581,7 +594,9 @@
       <c r="E4" s="1">
         <v>4</v>
       </c>
-      <c r="F4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="G4" s="1">
         <v>1</v>
       </c>
@@ -593,6 +608,9 @@
       </c>
       <c r="J4" s="1">
         <v>4</v>
+      </c>
+      <c r="K4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -611,6 +629,10 @@
       <c r="E5">
         <v>30.308581</v>
       </c>
+      <c r="F5">
+        <f>AVERAGE(B5:E5)</f>
+        <v>30.309357000000002</v>
+      </c>
       <c r="G5">
         <v>120.081059</v>
       </c>
@@ -622,6 +644,10 @@
       </c>
       <c r="J5">
         <v>120.08322699999999</v>
+      </c>
+      <c r="K5">
+        <f>AVERAGE(G5:J5)</f>
+        <v>120.08196049999998</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -640,6 +666,10 @@
       <c r="E6">
         <v>30.308933</v>
       </c>
+      <c r="F6">
+        <f t="shared" ref="F6:F25" si="0">AVERAGE(B6:E6)</f>
+        <v>30.309421749999998</v>
+      </c>
       <c r="G6">
         <v>120.08342</v>
       </c>
@@ -651,6 +681,10 @@
       </c>
       <c r="J6">
         <v>120.085544</v>
+      </c>
+      <c r="K6">
+        <f t="shared" ref="K6:K25" si="1">AVERAGE(G6:J6)</f>
+        <v>120.08436125</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -669,6 +703,10 @@
       <c r="E7">
         <v>30.307487999999999</v>
       </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>30.307835249999997</v>
+      </c>
       <c r="G7">
         <v>120.08116699999999</v>
       </c>
@@ -681,10 +719,14 @@
       <c r="J7">
         <v>120.083506</v>
       </c>
+      <c r="K7">
+        <f t="shared" si="1"/>
+        <v>120.08224249999999</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="B8">
         <v>30.307516</v>
@@ -698,6 +740,10 @@
       <c r="E8">
         <v>30.307891000000001</v>
       </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>30.308198000000001</v>
+      </c>
       <c r="G8">
         <v>120.083634</v>
       </c>
@@ -710,10 +756,14 @@
       <c r="J8">
         <v>120.085753</v>
       </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>120.0845905</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>30.309011999999999</v>
@@ -727,6 +777,10 @@
       <c r="E9">
         <v>30.309090999999999</v>
       </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>30.309683499999998</v>
+      </c>
       <c r="G9">
         <v>120.085705</v>
       </c>
@@ -739,10 +793,14 @@
       <c r="J9">
         <v>120.08639700000001</v>
       </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>120.08595450000001</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>30.307849999999998</v>
@@ -756,6 +814,10 @@
       <c r="E10">
         <v>30.307979</v>
       </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>30.30840525</v>
+      </c>
       <c r="G10">
         <v>120.085984</v>
       </c>
@@ -768,10 +830,14 @@
       <c r="J10">
         <v>120.087497</v>
       </c>
+      <c r="K10">
+        <f t="shared" si="1"/>
+        <v>120.08669875</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>30.309128000000001</v>
@@ -785,6 +851,10 @@
       <c r="E11">
         <v>30.309100000000001</v>
       </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>30.30937325</v>
+      </c>
       <c r="G11">
         <v>120.08824</v>
       </c>
@@ -797,10 +867,14 @@
       <c r="J11">
         <v>120.08874900000001</v>
       </c>
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>120.08850649999999</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>30.305057000000001</v>
@@ -814,6 +888,10 @@
       <c r="E12">
         <v>30.305482999999999</v>
       </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>30.306802749999999</v>
+      </c>
       <c r="G12">
         <v>120.08887799999999</v>
       </c>
@@ -826,10 +904,14 @@
       <c r="J12">
         <v>120.091517</v>
       </c>
+      <c r="K12">
+        <f t="shared" si="1"/>
+        <v>120.08984099999999</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>30.303353000000001</v>
@@ -843,6 +925,10 @@
       <c r="E13">
         <v>30.303417</v>
       </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>30.303808499999999</v>
+      </c>
       <c r="G13">
         <v>120.087988</v>
       </c>
@@ -855,10 +941,14 @@
       <c r="J13">
         <v>120.089162</v>
       </c>
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>120.0885845</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>30.301082999999998</v>
@@ -872,6 +962,10 @@
       <c r="E14">
         <v>30.300314</v>
       </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>30.301756749999999</v>
+      </c>
       <c r="G14">
         <v>120.088283</v>
       </c>
@@ -884,10 +978,14 @@
       <c r="J14">
         <v>120.09024599999999</v>
       </c>
+      <c r="K14">
+        <f t="shared" si="1"/>
+        <v>120.08917324999999</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>30.300211999999998</v>
@@ -901,6 +999,10 @@
       <c r="E15">
         <v>30.300243999999999</v>
       </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>30.300532499999996</v>
+      </c>
       <c r="G15">
         <v>120.08802900000001</v>
       </c>
@@ -913,10 +1015,14 @@
       <c r="J15">
         <v>120.09018</v>
       </c>
+      <c r="K15">
+        <f t="shared" si="1"/>
+        <v>120.08912050000001</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>30.300305000000002</v>
@@ -930,6 +1036,10 @@
       <c r="E16">
         <v>30.300277000000001</v>
       </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>30.301552749999999</v>
+      </c>
       <c r="G16">
         <v>120.09053400000001</v>
       </c>
@@ -942,10 +1052,14 @@
       <c r="J16">
         <v>120.09169300000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16">
+        <f t="shared" si="1"/>
+        <v>120.09104900000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17">
         <v>30.295974000000001</v>
@@ -959,6 +1073,10 @@
       <c r="E17">
         <v>30.295742000000001</v>
       </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>30.296430000000001</v>
+      </c>
       <c r="G17">
         <v>120.088238</v>
       </c>
@@ -971,10 +1089,14 @@
       <c r="J17">
         <v>120.092186</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17">
+        <f t="shared" si="1"/>
+        <v>120.090204</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B18">
         <v>30.297256999999998</v>
@@ -988,6 +1110,10 @@
       <c r="E18">
         <v>30.297201000000001</v>
       </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>30.297879999999999</v>
+      </c>
       <c r="G18">
         <v>120.088022</v>
       </c>
@@ -1000,10 +1126,14 @@
       <c r="J18">
         <v>120.08936300000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18">
+        <f t="shared" si="1"/>
+        <v>120.08868699999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19">
         <v>30.297201000000001</v>
@@ -1017,6 +1147,10 @@
       <c r="E19">
         <v>30.297173999999998</v>
       </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>30.298005</v>
+      </c>
       <c r="G19">
         <v>120.08949200000001</v>
       </c>
@@ -1029,10 +1163,14 @@
       <c r="J19">
         <v>120.092099</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19">
+        <f t="shared" si="1"/>
+        <v>120.09074450000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B20">
         <v>30.295423</v>
@@ -1046,6 +1184,10 @@
       <c r="E20">
         <v>30.295287999999999</v>
       </c>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>30.296176500000001</v>
+      </c>
       <c r="G20">
         <v>120.083365</v>
       </c>
@@ -1058,10 +1200,14 @@
       <c r="J20">
         <v>120.086611</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20">
+        <f t="shared" si="1"/>
+        <v>120.08495599999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B21">
         <v>30.297423999999999</v>
@@ -1075,6 +1221,10 @@
       <c r="E21">
         <v>30.297553000000001</v>
       </c>
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>30.298968250000001</v>
+      </c>
       <c r="G21">
         <v>120.08274299999999</v>
       </c>
@@ -1087,10 +1237,14 @@
       <c r="J21">
         <v>120.083955</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21">
+        <f t="shared" si="1"/>
+        <v>120.08323125</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B22">
         <v>30.30124</v>
@@ -1104,6 +1258,10 @@
       <c r="E22">
         <v>30.301203000000001</v>
       </c>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>30.3020575</v>
+      </c>
       <c r="G22">
         <v>120.084245</v>
       </c>
@@ -1116,10 +1274,14 @@
       <c r="J22">
         <v>120.085463</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22">
+        <f t="shared" si="1"/>
+        <v>120.08485125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B23">
         <v>30.301217000000001</v>
@@ -1133,6 +1295,10 @@
       <c r="E23">
         <v>30.301207999999999</v>
       </c>
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>30.302249750000001</v>
+      </c>
       <c r="G23">
         <v>120.08216899999999</v>
       </c>
@@ -1145,10 +1311,14 @@
       <c r="J23">
         <v>120.084132</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23">
+        <f t="shared" si="1"/>
+        <v>120.08307275</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B24">
         <v>30.304843999999999</v>
@@ -1162,6 +1332,10 @@
       <c r="E24">
         <v>30.305121</v>
       </c>
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>30.305239499999999</v>
+      </c>
       <c r="G24">
         <v>120.085581</v>
       </c>
@@ -1174,10 +1348,14 @@
       <c r="J24">
         <v>120.08754999999999</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24">
+        <f t="shared" si="1"/>
+        <v>120.08646199999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B25">
         <v>30.303629999999998</v>
@@ -1191,6 +1369,10 @@
       <c r="E25">
         <v>30.303823999999999</v>
       </c>
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>30.3039585</v>
+      </c>
       <c r="G25">
         <v>120.085796</v>
       </c>
@@ -1202,6 +1384,10 @@
       </c>
       <c r="J25">
         <v>120.08639700000001</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="1"/>
+        <v>120.08601350000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>